<commit_message>
[Document, Modified] : AddFriendsSpecification and MyChartSpecification
</commit_message>
<xml_diff>
--- a/ToDoApp-Doc/Document/Diagram/UseCase/AddFriends/AddFriendsSpecification.xlsx
+++ b/ToDoApp-Doc/Document/Diagram/UseCase/AddFriends/AddFriendsSpecification.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8355" activeTab="4"/>
+    <workbookView windowWidth="20385" windowHeight="8355" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Send Invitation" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59">
   <si>
     <t>Use-case number:</t>
   </si>
@@ -50,11 +50,14 @@
     <t>System response</t>
   </si>
   <si>
-    <t xml:space="preserve">- Người dùng nhấp vào "My friends"
+    <t xml:space="preserve"> - Người dùng nhấp vào "My friends"
+- Hệ thống hiển thị Friend List và nút "Add Friend"
 - Người dùng nhấp vào "Add friend"
+- Hệ thống hiển thị thanh tìm kiếm ID
 - Người dùng nhập user ID
-- Người dùng nhấn Enter
-</t>
+- Hệ thống hiển thị User ID
+- Người dùng nhấn Enter 
+- Hệ thống phản hồi cho người dùng biết họ đã gửi lời mời kết bạn cho tài khoản khác</t>
   </si>
   <si>
     <t>- Người dùng nhấp vào "My friends" 
@@ -105,7 +108,7 @@
     <t>Post-condition:</t>
   </si>
   <si>
-    <t>Nút thêm bạn bè đổi thành hủy lời mời kết bạn</t>
+    <t>Nút thêm bạn bè đổi thành hủy lời mời kết bạn. Đồng thời tài khoản được lưu vào danh sách bạn bè của người dùng</t>
   </si>
   <si>
     <t>View Friend List</t>
@@ -121,15 +124,18 @@
 - Hệ thống hiển thị Friend List</t>
   </si>
   <si>
+    <t xml:space="preserve"> - Người dùng nhấn vào "Friend List"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Hệ thống hiển thị danh sách bạn bè của người dùng</t>
+  </si>
+  <si>
+    <t>Không</t>
+  </si>
+  <si>
     <t>Người dùng nhấn vào "Friend List"</t>
   </si>
   <si>
-    <t>Hệ thống hiển thị danh sách bạn bè của người dùng</t>
-  </si>
-  <si>
-    <t>Không</t>
-  </si>
-  <si>
     <t>Người dùng phải kết bạn với tài khoản khác trước đó.</t>
   </si>
   <si>
@@ -142,11 +148,14 @@
     <t>Chức năng người dùng chia sẽ thành tựu cho bạn bè</t>
   </si>
   <si>
-    <t>- Người dùng nhấn vào "More activitive"
+    <t xml:space="preserve"> - Người dùng nhấn vào "More activitive"
+- Hệ thống hiển thị nút "More Activitive"
 - Người dùng nhấn vào
 biểu tượng thành tựu
+- Hệ thống hiển thị thành tựu của người dùng
 - Người dùng nhấn vào
-nút chia sẻ thành tựu</t>
+nút chia sẻ thành tựu
+- Hệ thống thông báo chia sẻ thành công</t>
   </si>
   <si>
     <t>- Người dùng nhấn vào "More Activitive"
@@ -165,7 +174,7 @@
     <t>Người dùng phải hoàn thành các nhiệm vụ đúng theo tiến độ đã thêm và sắp xếp trước đó</t>
   </si>
   <si>
-    <t>Hệ thống hiển thị các thành tựu của người dùng đã đạt được</t>
+    <t>Hệ thống hiển thị các thành tựu của người dùng đã đạt được. Đồng thời, thành tựu được chia sẻ đến cho bạn bè</t>
   </si>
   <si>
     <t>Unfriend</t>
@@ -201,7 +210,7 @@
     <t>Tài khoản muốn hủy kết bạn phải ở trạng thái bạn bè</t>
   </si>
   <si>
-    <t>Nút hủy kết bạn chuyển thành thêm bạn bè</t>
+    <t>Nút hủy kết bạn chuyển thành thêm bạn bè. Đồng thời tài khoản được lưu ở Friend List bị xóa đi</t>
   </si>
   <si>
     <t>Accept Invitation</t>
@@ -230,7 +239,7 @@
     <t>Phải có tài khoản khác gửi lời mời cho mình trước đó</t>
   </si>
   <si>
-    <t>Biểu tượng chấp nhận lời mời kết bạn chuyển thành biểu tượng hủy lời mời kết bạn</t>
+    <t>Biểu tượng chấp nhận lời mời kết bạn chuyển thành biểu tượng hủy lời mời kết bạn. Đồng thời tài khoản được lưu vào Friend List</t>
   </si>
 </sst>
 </file>
@@ -238,10 +247,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -276,28 +285,29 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -325,8 +335,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -340,9 +367,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -350,30 +384,36 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C0006"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F76"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C6500"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -394,37 +434,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -441,43 +450,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -487,146 +634,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -677,10 +686,38 @@
     </border>
     <border>
       <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -710,45 +747,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -773,18 +771,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -794,130 +816,130 @@
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -944,9 +966,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -954,7 +973,10 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -965,10 +987,10 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
@@ -1234,8 +1256,8 @@
   </sheetPr>
   <dimension ref="B2:D13"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="3"/>
@@ -1245,14 +1267,14 @@
     <col min="4" max="4" width="43.8571428571429" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4">
+    <row r="2" ht="32" customHeight="1" spans="2:4">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="12"/>
     </row>
-    <row r="3" spans="2:4">
+    <row r="3" ht="32" customHeight="1" spans="2:4">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1261,7 +1283,7 @@
       </c>
       <c r="D3" s="13"/>
     </row>
-    <row r="4" spans="2:4">
+    <row r="4" ht="32" customHeight="1" spans="2:4">
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1270,7 +1292,7 @@
       </c>
       <c r="D4" s="13"/>
     </row>
-    <row r="5" ht="31.5" spans="2:4">
+    <row r="5" ht="32" customHeight="1" spans="2:4">
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
@@ -1279,7 +1301,7 @@
       </c>
       <c r="D5" s="13"/>
     </row>
-    <row r="6" spans="2:4">
+    <row r="6" ht="32" customHeight="1" spans="2:4">
       <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1290,7 +1312,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" ht="110.25" spans="2:4">
+    <row r="7" ht="253" customHeight="1" spans="2:4">
       <c r="B7" s="6" t="s">
         <v>10</v>
       </c>
@@ -1301,16 +1323,16 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" ht="105" customHeight="1" spans="2:4">
+    <row r="8" ht="32" customHeight="1" spans="2:4">
       <c r="B8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="16"/>
-    </row>
-    <row r="9" spans="2:4">
+      <c r="D8" s="15"/>
+    </row>
+    <row r="9" ht="32" customHeight="1" spans="2:4">
       <c r="B9" s="1" t="s">
         <v>15</v>
       </c>
@@ -1319,7 +1341,7 @@
       </c>
       <c r="D9" s="13"/>
     </row>
-    <row r="10" ht="31.5" spans="2:4">
+    <row r="10" ht="32" customHeight="1" spans="2:4">
       <c r="B10" s="1" t="s">
         <v>17</v>
       </c>
@@ -1328,16 +1350,16 @@
       </c>
       <c r="D10" s="13"/>
     </row>
-    <row r="11" spans="2:4">
+    <row r="11" ht="32" customHeight="1" spans="2:4">
       <c r="B11" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="13"/>
-    </row>
-    <row r="12" spans="2:4">
+      <c r="D11" s="16"/>
+    </row>
+    <row r="12" ht="32" customHeight="1" spans="2:4">
       <c r="B12" s="1" t="s">
         <v>21</v>
       </c>
@@ -1346,7 +1368,7 @@
       </c>
       <c r="D12" s="13"/>
     </row>
-    <row r="13" ht="31.5" spans="2:4">
+    <row r="13" ht="32" customHeight="1" spans="2:4">
       <c r="B13" s="1" t="s">
         <v>23</v>
       </c>
@@ -1356,6 +1378,13 @@
       <c r="D13" s="13"/>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>
@@ -1368,8 +1397,8 @@
   </sheetPr>
   <dimension ref="B2:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="3"/>
@@ -1378,113 +1407,113 @@
     <col min="3" max="4" width="44" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4">
+    <row r="2" ht="32" customHeight="1" spans="2:4">
       <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="2:4">
+    <row r="3" ht="32" customHeight="1" spans="2:4">
       <c r="B3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="2:4">
+    <row r="4" ht="32" customHeight="1" spans="2:4">
       <c r="B4" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="9"/>
-    </row>
-    <row r="5" spans="2:4">
+      <c r="D4" s="8"/>
+    </row>
+    <row r="5" ht="32" customHeight="1" spans="2:4">
       <c r="B5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="2:4">
+    <row r="6" ht="32" customHeight="1" spans="2:4">
       <c r="B6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" ht="63" spans="2:4">
+    <row r="7" ht="92" customHeight="1" spans="2:4">
       <c r="B7" s="6" t="s">
         <v>28</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="2:4">
+    <row r="8" ht="32" customHeight="1" spans="2:4">
       <c r="B8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="2" t="s">
         <v>31</v>
       </c>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="2:4">
+    <row r="9" ht="32" customHeight="1" spans="2:4">
       <c r="B9" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="2:4">
+    <row r="10" ht="32" customHeight="1" spans="2:4">
       <c r="B10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="2" t="s">
         <v>31</v>
       </c>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="2:4">
+    <row r="11" ht="32" customHeight="1" spans="2:4">
       <c r="B11" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>29</v>
+      <c r="C11" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="2:4">
+    <row r="12" ht="32" customHeight="1" spans="2:4">
       <c r="B12" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>32</v>
+      <c r="C12" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="2:4">
+    <row r="13" ht="32" customHeight="1" spans="2:4">
       <c r="B13" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>33</v>
+      <c r="C13" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="D13" s="3"/>
     </row>
@@ -1512,8 +1541,8 @@
   </sheetPr>
   <dimension ref="B2:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="3"/>
@@ -1523,115 +1552,115 @@
     <col min="4" max="4" width="43.8571428571429" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4">
+    <row r="2" ht="32" customHeight="1" spans="2:4">
       <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="2:4">
+    <row r="3" ht="32" customHeight="1" spans="2:4">
       <c r="B3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>34</v>
+      <c r="C3" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="2:4">
+    <row r="4" ht="32" customHeight="1" spans="2:4">
       <c r="B4" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="9"/>
-    </row>
-    <row r="5" spans="2:4">
+      <c r="D4" s="8"/>
+    </row>
+    <row r="5" ht="32" customHeight="1" spans="2:4">
       <c r="B5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>35</v>
+      <c r="C5" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="2:4">
+    <row r="6" ht="32" customHeight="1" spans="2:4">
       <c r="B6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" ht="94.5" spans="2:4">
+    <row r="7" ht="207" customHeight="1" spans="2:4">
       <c r="B7" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7" s="10" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="8" spans="2:4">
+      <c r="D7" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" ht="32" customHeight="1" spans="2:4">
       <c r="B8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="2" t="s">
         <v>31</v>
       </c>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="2:4">
+    <row r="9" ht="32" customHeight="1" spans="2:4">
       <c r="B9" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="2:4">
+    <row r="10" ht="32" customHeight="1" spans="2:4">
       <c r="B10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="2" t="s">
         <v>31</v>
       </c>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="2:4">
+    <row r="11" ht="32" customHeight="1" spans="2:4">
       <c r="B11" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>39</v>
+      <c r="C11" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="2:4">
+    <row r="12" ht="32" customHeight="1" spans="2:4">
       <c r="B12" s="7" t="s">
         <v>21</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="2:4">
+    <row r="13" ht="32" customHeight="1" spans="2:4">
       <c r="B13" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="3"/>
+      <c r="C13" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -1657,8 +1686,8 @@
   </sheetPr>
   <dimension ref="B2:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="3"/>
@@ -1668,115 +1697,115 @@
     <col min="4" max="4" width="43.5714285714286" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4">
+    <row r="2" ht="32" customHeight="1" spans="2:4">
       <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="2:4">
+    <row r="3" ht="32" customHeight="1" spans="2:4">
       <c r="B3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>42</v>
+      <c r="C3" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="2:4">
+    <row r="4" ht="32" customHeight="1" spans="2:4">
       <c r="B4" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="9"/>
-    </row>
-    <row r="5" spans="2:4">
+      <c r="D4" s="8"/>
+    </row>
+    <row r="5" ht="32" customHeight="1" spans="2:4">
       <c r="B5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>43</v>
+      <c r="C5" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="2:4">
+    <row r="6" ht="32" customHeight="1" spans="2:4">
       <c r="B6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" ht="220.5" spans="2:4">
+    <row r="7" ht="252" customHeight="1" spans="2:4">
       <c r="B7" s="6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" s="10" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="8" spans="2:4">
+      <c r="D7" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" ht="32" customHeight="1" spans="2:4">
       <c r="B8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="2" t="s">
         <v>31</v>
       </c>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="2:4">
+    <row r="9" ht="32" customHeight="1" spans="2:4">
       <c r="B9" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="2:4">
+    <row r="10" ht="32" customHeight="1" spans="2:4">
       <c r="B10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="2" t="s">
         <v>31</v>
       </c>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="2:4">
+    <row r="11" ht="32" customHeight="1" spans="2:4">
       <c r="B11" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>47</v>
+      <c r="C11" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="2:4">
+    <row r="12" ht="32" customHeight="1" spans="2:4">
       <c r="B12" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>48</v>
+      <c r="C12" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="2:4">
+    <row r="13" ht="32" customHeight="1" spans="2:4">
       <c r="B13" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D13" s="3"/>
+      <c r="C13" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -1802,8 +1831,8 @@
   </sheetPr>
   <dimension ref="B2:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="3"/>
@@ -1813,23 +1842,23 @@
     <col min="4" max="4" width="43.4285714285714" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4">
+    <row r="2" ht="32" customHeight="1" spans="2:4">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="2:4">
+    <row r="3" ht="32" customHeight="1" spans="2:4">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="2:4">
+    <row r="4" ht="32" customHeight="1" spans="2:4">
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1838,16 +1867,16 @@
       </c>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="2:4">
+    <row r="5" ht="32" customHeight="1" spans="2:4">
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="2:4">
+    <row r="6" ht="32" customHeight="1" spans="2:4">
       <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1858,18 +1887,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" ht="141.75" spans="2:4">
+    <row r="7" ht="168" customHeight="1" spans="2:4">
       <c r="B7" s="6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" ht="32" customHeight="1" spans="2:4">
       <c r="B8" s="1" t="s">
         <v>13</v>
       </c>
@@ -1878,7 +1907,7 @@
       </c>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="2:4">
+    <row r="9" ht="32" customHeight="1" spans="2:4">
       <c r="B9" s="1" t="s">
         <v>15</v>
       </c>
@@ -1887,7 +1916,7 @@
       </c>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="2:4">
+    <row r="10" ht="32" customHeight="1" spans="2:4">
       <c r="B10" s="1" t="s">
         <v>17</v>
       </c>
@@ -1896,30 +1925,30 @@
       </c>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="2:4">
+    <row r="11" ht="32" customHeight="1" spans="2:4">
       <c r="B11" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="2:4">
+    <row r="12" ht="32" customHeight="1" spans="2:4">
       <c r="B12" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="2:4">
+    <row r="13" ht="32" customHeight="1" spans="2:4">
       <c r="B13" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D13" s="3"/>
     </row>

</xml_diff>